<commit_message>
Handle BangKeSuDungTienVay + UyNhiemChi
</commit_message>
<xml_diff>
--- a/adg-api/src/main/resources/viettin/bang-ke-su-dung-tien-vay.xlsx
+++ b/adg-api/src/main/resources/viettin/bang-ke-su-dung-tien-vay.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luan.phm/engineering/Projects/ADongGroup/adg-services-v2/adg-api/src/main/resources/viettin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{97822C51-652D-7542-A79E-2FAFF5AB1C21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7397A67B-4625-5E4E-BA4E-2A7371DF480E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34400" yWindow="460" windowWidth="34400" windowHeight="28340" xr2:uid="{7AA5DCE5-A5DB-5B4C-8DB7-F7DE94E7C3BC}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="34400" windowHeight="28340" xr2:uid="{7AA5DCE5-A5DB-5B4C-8DB7-F7DE94E7C3BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -65,23 +65,12 @@
     <t>MỤC ĐÍCH</t>
   </si>
   <si>
-    <t>SỐ
- CHỨNG TỪ</t>
-  </si>
-  <si>
     <t>NGÀY CHỨNG TỪ</t>
   </si>
   <si>
-    <t>SỐ TIỀN 
-(VND)</t>
-  </si>
-  <si>
     <t>SỐ TIỀN ĐÃ THANH TOÁN (VND)</t>
   </si>
   <si>
-    <t>SỐ TIỀN NHẬN NỢ  (VND)</t>
-  </si>
-  <si>
     <t>PHƯƠNG THỨC GIẢI NGÂN</t>
   </si>
   <si>
@@ -113,6 +102,15 @@
   </si>
   <si>
     <t xml:space="preserve">P. GIÁM ĐỐC </t>
+  </si>
+  <si>
+    <t>SỐ CHỨNG TỪ</t>
+  </si>
+  <si>
+    <t>SỐ TIỀN (VND)</t>
+  </si>
+  <si>
+    <t>SỐ TIỀN NHẬN NỢ (VND)</t>
   </si>
 </sst>
 </file>
@@ -293,7 +291,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -306,9 +304,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -326,123 +321,130 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -759,11 +761,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB517660-17F5-1F4D-9536-C5A840499E5F}">
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -772,6 +772,7 @@
     <col min="3" max="3" width="15.6640625" customWidth="1"/>
     <col min="4" max="4" width="27.33203125" customWidth="1"/>
     <col min="5" max="5" width="18.5" customWidth="1"/>
+    <col min="6" max="6" width="14.83203125" customWidth="1"/>
     <col min="8" max="8" width="13.6640625" customWidth="1"/>
     <col min="9" max="9" width="13.83203125" customWidth="1"/>
     <col min="10" max="10" width="13.6640625" customWidth="1"/>
@@ -795,242 +796,246 @@
       <c r="K1" s="5"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
       <c r="F2" s="5"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
       <c r="K2" s="5"/>
     </row>
     <row r="3" spans="1:11" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="13"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="12"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="49"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="49"/>
+      <c r="K4" s="49"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="16"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
+      <c r="A5" s="13"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
       <c r="K5" s="5"/>
     </row>
-    <row r="6" spans="1:11" ht="42" x14ac:dyDescent="0.2">
-      <c r="A6" s="19" t="s">
+    <row r="6" spans="1:11" s="44" customFormat="1" ht="42" x14ac:dyDescent="0.2">
+      <c r="A6" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="19" t="s">
+      <c r="F6" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="20" t="s">
+      <c r="H6" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="19" t="s">
+      <c r="J6" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="19" t="s">
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="18"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="45"/>
+      <c r="I7" s="55"/>
+      <c r="J7" s="41"/>
+      <c r="K7" s="18"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="J6" s="19" t="s">
+      <c r="B8" s="52"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="52"/>
+      <c r="F8" s="52"/>
+      <c r="G8" s="53"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="40"/>
+      <c r="K8" s="42"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="23"/>
+      <c r="B9" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="K6" s="19" t="s">
+      <c r="C9" s="24"/>
+      <c r="D9" s="25" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="21"/>
-      <c r="B7" s="21"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="50"/>
-      <c r="I7" s="24"/>
-      <c r="J7" s="52"/>
-      <c r="K7" s="21"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="26" t="s">
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="23"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="28"/>
+      <c r="B10" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="27"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="51"/>
-      <c r="I8" s="29"/>
-      <c r="J8" s="51"/>
-      <c r="K8" s="53"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="30"/>
-      <c r="B9" s="30" t="s">
+      <c r="C10" s="30"/>
+      <c r="D10" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="31"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="34"/>
+      <c r="J10" s="34"/>
+      <c r="K10" s="35"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="23"/>
+      <c r="B11" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="31"/>
-      <c r="D9" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="30"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="34"/>
-      <c r="J9" s="34"/>
-      <c r="K9" s="30"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="35"/>
-      <c r="B10" s="36" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="37"/>
-      <c r="D10" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="38"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="37"/>
-      <c r="I10" s="41"/>
-      <c r="J10" s="41"/>
-      <c r="K10" s="42"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="30"/>
-      <c r="B11" s="36" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="31"/>
-      <c r="D11" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" s="30"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="34"/>
-      <c r="J11" s="34"/>
-      <c r="K11" s="31"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="24"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="3"/>
-      <c r="C12" s="43"/>
+      <c r="C12" s="36"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="2"/>
       <c r="G12" s="4"/>
-      <c r="H12" s="44">
+      <c r="H12" s="54">
         <v>44710</v>
       </c>
-      <c r="I12" s="44"/>
-      <c r="J12" s="44"/>
+      <c r="I12" s="54"/>
+      <c r="J12" s="54"/>
       <c r="K12" s="5"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="45" t="s">
+      <c r="A13" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="46"/>
+      <c r="C13" s="46"/>
+      <c r="D13" s="46"/>
+      <c r="E13" s="46"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="46" t="s">
+        <v>2</v>
+      </c>
+      <c r="I13" s="46"/>
+      <c r="J13" s="46"/>
+      <c r="K13" s="38"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="46" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="46"/>
+      <c r="C14" s="39" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="45"/>
-      <c r="C13" s="45"/>
-      <c r="D13" s="45"/>
-      <c r="E13" s="45"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="46"/>
-      <c r="H13" s="45" t="s">
-        <v>2</v>
-      </c>
-      <c r="I13" s="45"/>
-      <c r="J13" s="45"/>
-      <c r="K13" s="47"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="45" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="45"/>
-      <c r="C14" s="48" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="49" t="s">
-        <v>24</v>
-      </c>
-      <c r="E14" s="49"/>
+      <c r="E14" s="47"/>
       <c r="F14" s="2"/>
       <c r="G14" s="4"/>
-      <c r="H14" s="45" t="s">
-        <v>25</v>
-      </c>
-      <c r="I14" s="45"/>
-      <c r="J14" s="45"/>
-      <c r="K14" s="47"/>
+      <c r="H14" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="I14" s="46"/>
+      <c r="J14" s="46"/>
+      <c r="K14" s="38"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B19" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="A8:G8"/>
-    <mergeCell ref="H12:J12"/>
-    <mergeCell ref="A13:E13"/>
-    <mergeCell ref="H13:J13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="H14:J14"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A8:G8"/>
+    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="H13:J13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add env to slack noti, handle date of Bang Ke Su Dung Tien Vay Vietin
</commit_message>
<xml_diff>
--- a/adg-api/src/main/resources/viettin/bang-ke-su-dung-tien-vay.xlsx
+++ b/adg-api/src/main/resources/viettin/bang-ke-su-dung-tien-vay.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luan.phm/engineering/Projects/ADongGroup/adg-services-v2/adg-api/src/main/resources/viettin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37C21C07-7019-E147-AEF0-B2DC674642E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D0F6520-1368-F242-81E3-4DDB55134B28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="34400" windowHeight="28340" xr2:uid="{7AA5DCE5-A5DB-5B4C-8DB7-F7DE94E7C3BC}"/>
   </bookViews>
@@ -416,6 +416,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -441,9 +444,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -763,7 +763,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB517660-17F5-1F4D-9536-C5A840499E5F}">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12:J12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -796,11 +798,11 @@
       <c r="K1" s="5"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="48"/>
-      <c r="C2" s="48"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
       <c r="F2" s="5"/>
@@ -826,19 +828,19 @@
       <c r="K3" s="12"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="49" t="s">
+      <c r="A4" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="49"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
-      <c r="F4" s="49"/>
-      <c r="G4" s="50"/>
-      <c r="H4" s="49"/>
-      <c r="I4" s="49"/>
-      <c r="J4" s="49"/>
-      <c r="K4" s="49"/>
+      <c r="B4" s="50"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="50"/>
+      <c r="I4" s="50"/>
+      <c r="J4" s="50"/>
+      <c r="K4" s="50"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="13"/>
@@ -896,21 +898,21 @@
       <c r="E7" s="18"/>
       <c r="F7" s="19"/>
       <c r="G7" s="20"/>
-      <c r="H7" s="55"/>
+      <c r="H7" s="46"/>
       <c r="I7" s="45"/>
       <c r="J7" s="41"/>
       <c r="K7" s="18"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="51" t="s">
+      <c r="A8" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="52"/>
-      <c r="C8" s="52"/>
-      <c r="D8" s="52"/>
-      <c r="E8" s="52"/>
-      <c r="F8" s="52"/>
-      <c r="G8" s="53"/>
+      <c r="B8" s="53"/>
+      <c r="C8" s="53"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="53"/>
+      <c r="F8" s="53"/>
+      <c r="G8" s="54"/>
       <c r="H8" s="40"/>
       <c r="I8" s="22"/>
       <c r="J8" s="40"/>
@@ -975,49 +977,49 @@
       <c r="E12" s="3"/>
       <c r="F12" s="2"/>
       <c r="G12" s="4"/>
-      <c r="H12" s="54">
+      <c r="H12" s="55">
         <v>44710</v>
       </c>
-      <c r="I12" s="54"/>
-      <c r="J12" s="54"/>
+      <c r="I12" s="55"/>
+      <c r="J12" s="55"/>
       <c r="K12" s="5"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="46" t="s">
+      <c r="A13" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="46"/>
-      <c r="C13" s="46"/>
-      <c r="D13" s="46"/>
-      <c r="E13" s="46"/>
+      <c r="B13" s="47"/>
+      <c r="C13" s="47"/>
+      <c r="D13" s="47"/>
+      <c r="E13" s="47"/>
       <c r="F13" s="1"/>
       <c r="G13" s="37"/>
-      <c r="H13" s="46" t="s">
+      <c r="H13" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="I13" s="46"/>
-      <c r="J13" s="46"/>
+      <c r="I13" s="47"/>
+      <c r="J13" s="47"/>
       <c r="K13" s="38"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="46" t="s">
+      <c r="A14" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="46"/>
+      <c r="B14" s="47"/>
       <c r="C14" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="47" t="s">
+      <c r="D14" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="E14" s="47"/>
+      <c r="E14" s="48"/>
       <c r="F14" s="2"/>
       <c r="G14" s="4"/>
-      <c r="H14" s="46" t="s">
+      <c r="H14" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="I14" s="46"/>
-      <c r="J14" s="46"/>
+      <c r="I14" s="47"/>
+      <c r="J14" s="47"/>
       <c r="K14" s="38"/>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.2">

</xml_diff>